<commit_message>
update logical model 800080629e233131db6c94e47e63653bef40085d
</commit_message>
<xml_diff>
--- a/ig/nr-test-log-model/StructureDefinition-log-cercle-de-soins.xlsx
+++ b/ig/nr-test-log-model/StructureDefinition-log-cercle-de-soins.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="101">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-14T08:58:47+00:00</t>
+    <t>2024-02-14T09:17:54+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -260,7 +260,7 @@
 </t>
   </si>
   <si>
-    <t>test</t>
+    <t>Identifiant du cercle de soins.</t>
   </si>
   <si>
     <t>log-cercle-de-soins.dateCreation</t>
@@ -270,13 +270,22 @@
 </t>
   </si>
   <si>
+    <t>Date de création du cercle de soin.</t>
+  </si>
+  <si>
     <t>log-cercle-de-soins.dateMAJ</t>
   </si>
   <si>
+    <t>Date de mise à jour du cercle de soin.</t>
+  </si>
+  <si>
     <t>Le concept de cercle de soins a plusieurs dates de mise à jour mais chaque version de la ressource, et donc chaque instance de la ressource, ne peut avoir qu’une seule date de mise à jour</t>
   </si>
   <si>
     <t>log-cercle-de-soins.dateFin</t>
+  </si>
+  <si>
+    <t>Date de fin d'existence du cercle de soins.</t>
   </si>
   <si>
     <t>log-cercle-de-soins.statut</t>
@@ -286,11 +295,33 @@
 </t>
   </si>
   <si>
+    <t>Statut du cercle de soins.</t>
+  </si>
+  <si>
+    <t>La liste des valeurs possibles n'est pas définie par ces spécifications. Les codes possibles ainsi que le sens donné sont définis par le gestionnaire en fonction du projet. Il peut s'inspirer du jeu de valeur FHIR CareTeamStatus (proposed | active | suspended | inactive | entered-in-error).]]</t>
+  </si>
+  <si>
     <t>log-cercle-de-soins.metadonnee</t>
   </si>
   <si>
     <t xml:space="preserve">Meta
 </t>
+  </si>
+  <si>
+    <t>Informations relatives à la gestion des classes et des données.</t>
+  </si>
+  <si>
+    <t>log-cercle-de-soins.PersonnePriseCharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://interop.esante.gouv.fr/ig/fhir/cds/StructureDefinition/log-personne-prise-charge
+</t>
+  </si>
+  <si>
+    <t>Personne prise en charge.</t>
+  </si>
+  <si>
+    <t>La personne prise en charge.</t>
   </si>
 </sst>
 </file>
@@ -595,7 +626,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK8"/>
+  <dimension ref="A1:AK9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -604,8 +635,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="31.328125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="31.328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="38.515625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="38.515625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="8.95703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
@@ -614,7 +645,7 @@
     <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="9.3046875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="79.71875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -635,7 +666,7 @@
     <col min="29" max="29" width="20.59375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="31.328125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="38.515625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
@@ -992,10 +1023,10 @@
         <v>83</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -1066,10 +1097,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -1095,10 +1126,10 @@
         <v>83</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1149,7 +1180,7 @@
         <v>73</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>79</v>
@@ -1169,10 +1200,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
@@ -1198,10 +1229,10 @@
         <v>83</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1252,7 +1283,7 @@
         <v>73</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>74</v>
@@ -1272,10 +1303,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
@@ -1298,13 +1329,13 @@
         <v>73</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1355,7 +1386,7 @@
         <v>73</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>74</v>
@@ -1375,10 +1406,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
@@ -1401,13 +1432,13 @@
         <v>73</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -1458,7 +1489,7 @@
         <v>73</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="AG8" t="s" s="2">
         <v>79</v>
@@ -1473,6 +1504,109 @@
         <v>73</v>
       </c>
       <c r="AK8" t="s" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="G9" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="I9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="J9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="K9" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="L9" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="M9" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Q9" s="2"/>
+      <c r="R9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="S9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="T9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="U9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="V9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="W9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="X9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Y9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="Z9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AA9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AB9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AC9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AD9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AE9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AF9" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="AG9" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AH9" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AJ9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AK9" t="s" s="2">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add professionnel & exercice professionnel bb8691095d4c835bebf2cb6515ffb91f6cf27e49
</commit_message>
<xml_diff>
--- a/ig/nr-test-log-model/StructureDefinition-log-cercle-de-soins.xlsx
+++ b/ig/nr-test-log-model/StructureDefinition-log-cercle-de-soins.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="114">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-14T09:42:21+00:00</t>
+    <t>2024-02-14T17:54:26+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -349,6 +349,19 @@
   </si>
   <si>
     <t>subject</t>
+  </si>
+  <si>
+    <t>log-cercle-de-soins.MembreCercleSoin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://interop.esante.gouv.fr/ig/fhir/cds/StructureDefinition/log-membre-cercle-de-soins
+</t>
+  </si>
+  <si>
+    <t>Membre du cercle de soin</t>
+  </si>
+  <si>
+    <t>participant.member</t>
   </si>
 </sst>
 </file>
@@ -653,7 +666,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL9"/>
+  <dimension ref="A1:AL10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -672,7 +685,7 @@
     <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="79.71875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="81.234375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1665,6 +1678,112 @@
         <v>109</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G10" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="K10" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="L10" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="M10" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF10" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AG10" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH10" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK10" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL10" t="s" s="2">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>